<commit_message>
fixed q2 part a and made sure all code runs, ready for turn in
</commit_message>
<xml_diff>
--- a/partB_q2_KNN.xlsx
+++ b/partB_q2_KNN.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manor\Desktop\University\Semester6\IntroArtificialInt\hw\ai_hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44D7B5C-14FD-47A6-A572-F41ECB2737EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9726BF-10B9-4189-B210-43DDA5E485A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="q2_1" sheetId="1" r:id="rId1"/>
     <sheet name="q2_2" sheetId="2" r:id="rId2"/>
+    <sheet name="q2_3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -239,13 +240,13 @@
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9000000000000004</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
@@ -272,13 +273,13 @@
                   <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9000000000000004</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5</c:v>
@@ -590,7 +591,1628 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="dash"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-E067-497C-9D38-133C119A7255}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-E067-497C-9D38-133C119A7255}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-E067-497C-9D38-133C119A7255}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-E067-497C-9D38-133C119A7255}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="dash"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-E067-497C-9D38-133C119A7255}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="dash"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-E067-497C-9D38-133C119A7255}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>q2_1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>q2_1!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E067-497C-9D38-133C119A7255}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="515128447"/>
+        <c:axId val="515130527"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="515128447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>v1</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="515130527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="515130527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>v2</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="515128447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-AB2A-4F34-8C00-CA7E53670BBF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-AB2A-4F34-8C00-CA7E53670BBF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>q2_2!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>q2_2!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AB2A-4F34-8C00-CA7E53670BBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="138895071"/>
+        <c:axId val="133009007"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="138895071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>v1</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="133009007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="133009007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>v2</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="138895071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="dash"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-50C9-4A60-8FF3-32CD0F5774B5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-50C9-4A60-8FF3-32CD0F5774B5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-50C9-4A60-8FF3-32CD0F5774B5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-50C9-4A60-8FF3-32CD0F5774B5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="dash"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-50C9-4A60-8FF3-32CD0F5774B5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>q2_3!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>q2_3!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-50C9-4A60-8FF3-32CD0F5774B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="434408623"/>
+        <c:axId val="434410703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="434408623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>v1</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="434410703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="434410703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>v2</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="434408623"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1146,6 +2768,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1167,6 +4337,124 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B24E561-5C15-44E2-A73C-18F9A61B8DA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04EAD29F-051C-4DAD-BFA0-83C6C957915F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>109537</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{536FB0C1-2FF9-4286-B558-D94A117143AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>395287</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{180EE0F3-8C17-4A00-9B16-C44F4B42D468}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1452,8 +4740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,7 +4778,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4.9000000000000004</v>
+        <v>5.6</v>
       </c>
       <c r="B5">
         <v>5.6</v>
@@ -1501,10 +4789,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
       <c r="B6">
-        <v>4.9000000000000004</v>
+        <v>5.7</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -1512,10 +4800,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1526,7 +4814,7 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1552,14 +4840,112 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B177198F-7EAA-43EF-9BDF-4742CB993782}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F192F9-0714-4BDE-AB23-B3600ADF69F4}">
+  <dimension ref="A2:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>